<commit_message>
62801- Fixed AdultFundingClaimReport template grouping formula
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR1819.ReportService.Stateless/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR1819.ReportService.Stateless/AdultFundingClaimReportTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DDA6EA-7299-4494-B507-19BBBF31D2BD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40677E1A-BC63-4878-B299-908EA0AF4BE7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -587,17 +587,35 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
@@ -643,24 +661,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1377,24 +1377,24 @@
   <dimension ref="B2:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="4" customWidth="1"/>
-    <col min="6" max="7" width="20.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="2.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="3.1328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.73046875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.86328125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.86328125" style="4" customWidth="1"/>
+    <col min="6" max="7" width="20.73046875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="6.265625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="2.265625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.1328125" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9.1328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1402,28 +1402,28 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="45" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" ht="20.65" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="8"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="42"/>
+      <c r="J3" s="40"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1431,9 +1431,9 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
-      <c r="J4" s="42"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="J4" s="40"/>
+    </row>
+    <row r="5" spans="2:16" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="12" t="s">
         <v>0</v>
@@ -1444,9 +1444,9 @@
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="42"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="J5" s="40"/>
+    </row>
+    <row r="6" spans="2:16" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="12" t="s">
         <v>1</v>
@@ -1457,9 +1457,9 @@
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="42"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="J6" s="40"/>
+    </row>
+    <row r="7" spans="2:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B7" s="5"/>
       <c r="C7" s="12" t="s">
         <v>2</v>
@@ -1472,9 +1472,9 @@
       <c r="G7" s="39"/>
       <c r="H7" s="8"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="42"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="J7" s="40"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -1482,31 +1482,31 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="11"/>
-      <c r="J8" s="43"/>
-    </row>
-    <row r="9" spans="2:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="41"/>
+    </row>
+    <row r="9" spans="2:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="11"/>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -1514,15 +1514,15 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>
-      <c r="J10" s="45"/>
-    </row>
-    <row r="11" spans="2:16" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="50"/>
+    </row>
+    <row r="11" spans="2:16" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
       <c r="F11" s="17" t="s">
         <v>30</v>
       </c>
@@ -1530,79 +1530,79 @@
         <v>31</v>
       </c>
       <c r="H11" s="11"/>
-      <c r="J11" s="45"/>
-    </row>
-    <row r="12" spans="2:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="2:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="11"/>
-      <c r="J12" s="45"/>
+      <c r="J12" s="50"/>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="2:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="50"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="55"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
       <c r="H13" s="11"/>
-      <c r="J13" s="45"/>
+      <c r="J13" s="50"/>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="55"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
       <c r="H14" s="11"/>
-      <c r="J14" s="45"/>
+      <c r="J14" s="50"/>
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="50"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="55"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="11"/>
-      <c r="J15" s="45"/>
+      <c r="J15" s="50"/>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
       <c r="H16" s="11"/>
-      <c r="J16" s="45"/>
+      <c r="J16" s="50"/>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
       <c r="C17" s="36"/>
       <c r="D17" s="37"/>
@@ -1610,29 +1610,29 @@
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="H17" s="11"/>
-      <c r="J17" s="45"/>
+      <c r="J17" s="50"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="23">
-        <f>SUM(F14:F16)</f>
+        <f>SUM(F12:F16)</f>
         <v>0</v>
       </c>
       <c r="G18" s="23">
-        <f>SUM(G14:G16)</f>
+        <f>SUM(G12:G16)</f>
         <v>0</v>
       </c>
       <c r="H18" s="11"/>
-      <c r="J18" s="45"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J18" s="50"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1640,15 +1640,15 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="11"/>
-      <c r="J19" s="45"/>
-    </row>
-    <row r="20" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J19" s="50"/>
+    </row>
+    <row r="20" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="54"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
       <c r="F20" s="17" t="s">
         <v>32</v>
       </c>
@@ -1656,45 +1656,45 @@
         <v>31</v>
       </c>
       <c r="H20" s="11"/>
-      <c r="J20" s="45"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J20" s="50"/>
+    </row>
+    <row r="21" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
       <c r="H21" s="11"/>
-      <c r="J21" s="45"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J21" s="50"/>
+    </row>
+    <row r="22" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B22" s="5"/>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="60"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="44"/>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
       <c r="H22" s="11"/>
-      <c r="J22" s="45"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J22" s="50"/>
+    </row>
+    <row r="23" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
-      <c r="C23" s="58" t="s">
+      <c r="C23" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="60"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
       <c r="H23" s="11"/>
-      <c r="J23" s="45"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J23" s="50"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
       <c r="C24" s="20"/>
       <c r="D24" s="25"/>
@@ -1702,17 +1702,17 @@
       <c r="F24" s="26"/>
       <c r="G24" s="27"/>
       <c r="H24" s="11"/>
-      <c r="J24" s="45"/>
+      <c r="J24" s="50"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
-      <c r="C25" s="58" t="s">
+      <c r="C25" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="44"/>
       <c r="F25" s="23">
         <f>SUM(F21:F23)</f>
         <v>0</v>
@@ -1722,9 +1722,9 @@
         <v>0</v>
       </c>
       <c r="H25" s="11"/>
-      <c r="J25" s="45"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J25" s="50"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -1732,9 +1732,9 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="11"/>
-      <c r="J26" s="46"/>
-    </row>
-    <row r="27" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="51"/>
+    </row>
+    <row r="27" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1742,11 +1742,11 @@
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="11"/>
-      <c r="J27" s="41" t="s">
+      <c r="J27" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="5"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1754,9 +1754,9 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="11"/>
-      <c r="J28" s="42"/>
-    </row>
-    <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="40"/>
+    </row>
+    <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -1764,9 +1764,9 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="11"/>
-      <c r="J29" s="42"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J29" s="40"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="5"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -1774,9 +1774,9 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="11"/>
-      <c r="J30" s="42"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J30" s="40"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -1784,9 +1784,9 @@
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="11"/>
-      <c r="J31" s="42"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J31" s="40"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1794,9 +1794,9 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="11"/>
-      <c r="J32" s="42"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J32" s="40"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -1804,9 +1804,9 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="11"/>
-      <c r="J33" s="42"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J33" s="40"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" s="5"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -1814,9 +1814,9 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="11"/>
-      <c r="J34" s="43"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J34" s="41"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1824,11 +1824,11 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="11"/>
-      <c r="J35" s="42" t="s">
+      <c r="J35" s="40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="28" t="s">
         <v>14</v>
       </c>
@@ -1839,9 +1839,9 @@
       </c>
       <c r="F36" s="29"/>
       <c r="H36" s="30"/>
-      <c r="J36" s="42"/>
-    </row>
-    <row r="37" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J36" s="40"/>
+    </row>
+    <row r="37" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="28" t="s">
         <v>17</v>
       </c>
@@ -1852,9 +1852,9 @@
       </c>
       <c r="F37" s="29"/>
       <c r="H37" s="30"/>
-      <c r="J37" s="42"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J37" s="40"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" s="28" t="s">
         <v>20</v>
       </c>
@@ -1867,9 +1867,9 @@
       <c r="G38" s="29"/>
       <c r="H38" s="30"/>
       <c r="I38" s="29"/>
-      <c r="J38" s="42"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J38" s="40"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" s="28"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
@@ -1880,22 +1880,22 @@
       <c r="G39" s="29"/>
       <c r="H39" s="30"/>
       <c r="I39" s="29"/>
-      <c r="J39" s="42"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="61" t="s">
+      <c r="J39" s="40"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B40" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="62"/>
+      <c r="C40" s="47"/>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
       <c r="H40" s="32"/>
       <c r="I40" s="33"/>
-      <c r="J40" s="42"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J40" s="40"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41" s="34"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -1903,17 +1903,10 @@
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
       <c r="H41" s="35"/>
-      <c r="J41" s="43"/>
+      <c r="J41" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J35:J41"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="J27:J34"/>
-    <mergeCell ref="B40:C40"/>
     <mergeCell ref="K9:P9"/>
     <mergeCell ref="J2:J8"/>
     <mergeCell ref="J9:J26"/>
@@ -1927,12 +1920,16 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C18:E18"/>
+    <mergeCell ref="J35:J41"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="J27:J34"/>
+    <mergeCell ref="B40:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="F25:G25" unlockedFormula="1"/>
-  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>